<commit_message>
Added SWL, removed SAA
</commit_message>
<xml_diff>
--- a/data/dots_test_def.xlsx
+++ b/data/dots_test_def.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\dots_home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C8E5C9-C417-421B-B5CA-0F798D9B47A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03812BD2-6851-4C35-98C0-2692A3910313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="3285" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="516">
   <si>
     <t>name</t>
   </si>
@@ -2085,6 +2085,36 @@
   </si>
   <si>
     <t>https://link.springer.com/article/10.3758/s13428-019-01225-1</t>
+  </si>
+  <si>
+    <t>SWL</t>
+  </si>
+  <si>
+    <t>Satisfaction with Life (for Children)</t>
+  </si>
+  <si>
+    <t>Fragebogen zu Lebenszufriedenheit</t>
+  </si>
+  <si>
+    <t>en,de,lv</t>
+  </si>
+  <si>
+    <t>This measure life satisfaction</t>
+  </si>
+  <si>
+    <t>Misst Lebenszufriedenheit</t>
+  </si>
+  <si>
+    <t>http://testing.musikpsychologie.de/dots_demo_demo/?test=SWL</t>
+  </si>
+  <si>
+    <t>Gadermann, A. M., Schonert-Reichl, K. A., &amp; Zumbo, B. D. (2010). Investigating validity evidence of the Satisfaction With Life Scale adapted for children. Social Indicators Research, 96, 229-247</t>
+  </si>
+  <si>
+    <t>doi:10.1007/s11205-009-9474-1</t>
+  </si>
+  <si>
+    <t>Lang, J., &amp; Schmitz, B. (2020). German Translation of the Satisfaction With Life Scale for Children and Adolescents. Journal of Psychoeducational Assessment, 38(3), 291-304.</t>
   </si>
 </sst>
 </file>
@@ -2737,9 +2767,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R63" sqref="R63"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O99" sqref="O99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6433,7 +6463,7 @@
       <c r="N89" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="O89" s="5" t="s">
+      <c r="O89" s="7" t="s">
         <v>392</v>
       </c>
       <c r="P89" s="19" t="s">
@@ -6574,6 +6604,56 @@
       </c>
       <c r="R92" s="25" t="s">
         <v>483</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18">
+      <c r="A93" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="I93" s="1">
+        <v>5</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N93" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="O93" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="P93" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="Q93" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="R93" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="96" spans="1:18">
@@ -6759,6 +6839,7 @@
     <hyperlink ref="R70" r:id="rId80" xr:uid="{BF99CB95-8732-461D-BBA6-6F0D17CAFA88}"/>
     <hyperlink ref="R55" r:id="rId81" xr:uid="{448C4D42-C0A1-4722-8FE4-D98BC3811EC5}"/>
     <hyperlink ref="R63" r:id="rId82" xr:uid="{46EABFE7-A6DC-474E-939A-50AFAA4C570B}"/>
+    <hyperlink ref="N93" r:id="rId83" xr:uid="{86C37DF7-FE20-484C-B894-B49330FE0034}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>